<commit_message>
variables listas menos diagnosticos
</commit_message>
<xml_diff>
--- a/DICCIONARIO_BD_URGENCIAS_BIO.xlsx
+++ b/DICCIONARIO_BD_URGENCIAS_BIO.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asv\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udeaeduco-my.sharepoint.com/personal/isabel_garcesg_udea_edu_co/Documents/UdeA/Semestre 9/Informatica medica/final/Final_project_ML/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64D5BE4-42E7-4BDA-A27E-28581B9C069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -946,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D3AC4C-4937-2842-B989-9D005DCF3100}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>